<commit_message>
Added burden Set critical path flag Removed IO operations
</commit_message>
<xml_diff>
--- a/docs/diss/write_up/results/spreadsheets/rectmul_speedup.xlsx
+++ b/docs/diss/write_up/results/spreadsheets/rectmul_speedup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="0" windowWidth="24480" windowHeight="16360" tabRatio="500"/>
+    <workbookView xWindow="620" yWindow="0" windowWidth="24480" windowHeight="16360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="dedup" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -226,14 +226,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -278,6 +281,7 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -322,6 +326,7 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1261,11 +1266,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2134042648"/>
-        <c:axId val="-2134195912"/>
+        <c:axId val="-2059299016"/>
+        <c:axId val="-2059295880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2134042648"/>
+        <c:axId val="-2059299016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1275,12 +1280,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134195912"/>
+        <c:crossAx val="-2059295880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2134195912"/>
+        <c:axId val="-2059295880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1291,7 +1296,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134042648"/>
+        <c:crossAx val="-2059299016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2471,11 +2476,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2138483288"/>
-        <c:axId val="-2138357640"/>
+        <c:axId val="-2058196968"/>
+        <c:axId val="-2058193896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2138483288"/>
+        <c:axId val="-2058196968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2485,12 +2490,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2138357640"/>
+        <c:crossAx val="-2058193896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2138357640"/>
+        <c:axId val="-2058193896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2501,7 +2506,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2138483288"/>
+        <c:crossAx val="-2058196968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3534,11 +3539,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2133064312"/>
-        <c:axId val="2132992920"/>
+        <c:axId val="-2058149720"/>
+        <c:axId val="-2058141560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2133064312"/>
+        <c:axId val="-2058149720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3567,12 +3572,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132992920"/>
+        <c:crossAx val="-2058141560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2132992920"/>
+        <c:axId val="-2058141560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3602,7 +3607,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133064312"/>
+        <c:crossAx val="-2058149720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4082,7 +4087,7 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4602,6 +4607,15 @@
       </c>
     </row>
     <row r="11" spans="1:18">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>32</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
       <c r="F11">
         <v>10</v>
       </c>
@@ -4654,6 +4668,15 @@
       </c>
     </row>
     <row r="12" spans="1:18">
+      <c r="C12" s="4">
+        <v>12795600</v>
+      </c>
+      <c r="D12" s="4">
+        <v>6936210</v>
+      </c>
+      <c r="E12" s="4">
+        <v>6029290</v>
+      </c>
       <c r="F12">
         <v>11</v>
       </c>
@@ -4706,6 +4729,14 @@
       </c>
     </row>
     <row r="13" spans="1:18">
+      <c r="D13">
+        <f>C12/D12</f>
+        <v>1.8447538353077546</v>
+      </c>
+      <c r="E13">
+        <f>C12/E12</f>
+        <v>2.1222399320649696</v>
+      </c>
       <c r="F13">
         <v>12</v>
       </c>

</xml_diff>